<commit_message>
updated tables to v20211116
Added minimum dissolved oxygen and ultimate biochemical oxygen demand to the list of pollutants for the Pudding TMDL (action ID 2037).
</commit_message>
<xml_diff>
--- a/data_raw/TMDL_db_tabular.xlsx
+++ b/data_raw/TMDL_db_tabular.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Planning statewide\TMDL_DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GitHub\odeqtmdl\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="555" yWindow="780" windowWidth="27075" windowHeight="13905"/>
+    <workbookView xWindow="555" yWindow="780" windowWidth="27075" windowHeight="13905" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tmdl_actions_table" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="552">
   <si>
     <t>Total Phosphorus</t>
   </si>
@@ -1385,9 +1385,6 @@
     <t>Total Phosphorus, BOD5, Ammonia</t>
   </si>
   <si>
-    <t>CBOD5, Total Suspended Solids, Ammonia Nitrogen (NH3-N)</t>
-  </si>
-  <si>
     <t>CBOD5, Ammonia Nitrogen (NH3-N)</t>
   </si>
   <si>
@@ -1397,15 +1394,6 @@
     <t>BOD</t>
   </si>
   <si>
-    <t>pH, Dissolved Oxygen, Nutrients, Periphyton, Temperature</t>
-  </si>
-  <si>
-    <t>Dissoloved ortho phosphate as phosphorus (PO4-P), Ammonia</t>
-  </si>
-  <si>
-    <t>Algae, pH, Bacteria (water contact recreation), DDT/DDE, dieldrin, dioxin, PCBs, Dissolved Oxygen, Lead</t>
-  </si>
-  <si>
     <t>Total Phosphorus, E. coli, DDT/DDE, dieldrin, dioxin, PCBs, BOD5, Lead</t>
   </si>
   <si>
@@ -1508,9 +1496,6 @@
     <t>Bacteria (water contact recreation), Dissolved Oxygen, Chlorophyll a, pH, Temperature</t>
   </si>
   <si>
-    <t>E. coli, fecal coliform, Total Phopshorus, Heat</t>
-  </si>
-  <si>
     <t>Bacteria (water contact recreation), Dissolved Oxygen, Temperature</t>
   </si>
   <si>
@@ -1680,6 +1665,30 @@
   </si>
   <si>
     <t>All 303(d) water quality limited parameters being addressed by the TMDL action.</t>
+  </si>
+  <si>
+    <t>pH, Dissolved Oxygen, Periphyton Growth, Ammonia Toxicity</t>
+  </si>
+  <si>
+    <t>Algae, pH, Bacteria (water contact recreation), Total Phosphorus, DDT/DDE, dieldrin, dioxin, PCBs, Dissolved Oxygen, Lead</t>
+  </si>
+  <si>
+    <t>v20211116</t>
+  </si>
+  <si>
+    <t>CBOD5, Total Suspended Solids, Ammonia Nitrogen (NH3-N), minimum dissolved oxygen, Ultimate Biochemical Oxygen Demand</t>
+  </si>
+  <si>
+    <t>Dissolved orthophosphate as phosphorus (PO4-P), Ammonia</t>
+  </si>
+  <si>
+    <t>E. coli, fecal coliform, Total Phosphorus, Heat</t>
+  </si>
+  <si>
+    <t>2037</t>
+  </si>
+  <si>
+    <t>Added minimum dissolved oxygen and ultimate biochemical oxygen demand to the list of pollutants for the Pudding TMDL (action ID 2037).</t>
   </si>
 </sst>
 </file>
@@ -1783,7 +1792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1901,7 +1910,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2184,8 +2192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,7 +2209,7 @@
     <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="50.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="69.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2221,13 +2229,13 @@
         <v>406</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>423</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>420</v>
@@ -2236,10 +2244,10 @@
         <v>436</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2259,13 +2267,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I2" s="26">
         <v>32408</v>
@@ -2301,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I3" s="28">
         <v>32408</v>
@@ -2337,7 +2345,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I4" s="28">
         <v>33294</v>
@@ -2373,7 +2381,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I5" s="26">
         <v>33462</v>
@@ -2401,12 +2409,15 @@
       <c r="D6" s="2" t="s">
         <v>430</v>
       </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
       <c r="F6" s="22"/>
       <c r="G6" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I6" s="28">
         <v>33462</v>
@@ -2442,7 +2453,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I7" s="28">
         <v>33462</v>
@@ -2451,15 +2462,15 @@
         <v>33679</v>
       </c>
       <c r="K7" s="33" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="L7" s="38" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="24">
-        <v>2037</v>
+      <c r="A8" s="24" t="s">
+        <v>550</v>
       </c>
       <c r="B8" t="s">
         <v>362</v>
@@ -2478,7 +2489,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I8" s="28">
         <v>34182</v>
@@ -2490,7 +2501,7 @@
         <v>61</v>
       </c>
       <c r="L8" s="35" t="s">
-        <v>450</v>
+        <v>547</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2514,7 +2525,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I9" s="28">
         <v>34304</v>
@@ -2526,7 +2537,7 @@
         <v>61</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -2546,13 +2557,13 @@
         <v>0</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I10" s="26">
         <v>34330</v>
@@ -2561,7 +2572,7 @@
         <v>34361</v>
       </c>
       <c r="K10" s="33" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L10" s="39" t="s">
         <v>0</v>
@@ -2588,7 +2599,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I11" s="28">
         <v>34394</v>
@@ -2600,7 +2611,7 @@
         <v>61</v>
       </c>
       <c r="L11" s="40" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2624,7 +2635,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I12" s="26">
         <v>34974</v>
@@ -2633,10 +2644,10 @@
         <v>35202</v>
       </c>
       <c r="K12" s="33" t="s">
-        <v>454</v>
+        <v>544</v>
       </c>
       <c r="L12" s="38" t="s">
-        <v>455</v>
+        <v>548</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -2660,7 +2671,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I13" s="26">
         <v>36039</v>
@@ -2669,10 +2680,10 @@
         <v>36124</v>
       </c>
       <c r="K13" s="33" t="s">
-        <v>456</v>
+        <v>545</v>
       </c>
       <c r="L13" s="40" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2696,7 +2707,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I14" s="26">
         <v>36220</v>
@@ -2708,7 +2719,7 @@
         <v>83</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2732,7 +2743,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I15" s="26">
         <v>36617</v>
@@ -2741,10 +2752,10 @@
         <v>36649</v>
       </c>
       <c r="K15" s="33" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="L15" s="35" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2768,7 +2779,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I16" s="26">
         <v>36892</v>
@@ -2780,7 +2791,7 @@
         <v>83</v>
       </c>
       <c r="L16" s="22" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -2804,7 +2815,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I17" s="26">
         <v>36951</v>
@@ -2813,10 +2824,10 @@
         <v>37020</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="L17" s="35" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2840,7 +2851,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I18" s="26">
         <v>37043</v>
@@ -2849,10 +2860,10 @@
         <v>37103</v>
       </c>
       <c r="K18" s="33" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="L18" s="22" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2876,7 +2887,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I19" s="26">
         <v>37104</v>
@@ -2885,7 +2896,7 @@
         <v>37110</v>
       </c>
       <c r="K19" s="33" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="L19" s="22" t="s">
         <v>0</v>
@@ -2912,7 +2923,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I20" s="26">
         <v>37226</v>
@@ -2921,10 +2932,10 @@
         <v>37285</v>
       </c>
       <c r="K20" s="33" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="L20" s="40" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -2944,13 +2955,13 @@
         <v>0</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I21" s="26">
         <v>37226</v>
@@ -2962,7 +2973,7 @@
         <v>83</v>
       </c>
       <c r="L21" s="22" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2986,7 +2997,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I22" s="26">
         <v>37347</v>
@@ -2998,7 +3009,7 @@
         <v>83</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -3022,7 +3033,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I23" s="26">
         <v>37347</v>
@@ -3034,7 +3045,7 @@
         <v>83</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3058,7 +3069,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I24" s="26">
         <v>37347</v>
@@ -3067,10 +3078,10 @@
         <v>37389</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="L24" s="40" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -3094,7 +3105,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I25" s="26">
         <v>37377</v>
@@ -3103,10 +3114,10 @@
         <v>37475</v>
       </c>
       <c r="K25" s="33" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="L25" s="22" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -3120,7 +3131,7 @@
         <v>2002</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
@@ -3130,7 +3141,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I26" s="26">
         <v>37526</v>
@@ -3139,10 +3150,10 @@
         <v>37578</v>
       </c>
       <c r="K26" s="33" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="L26" s="41" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3156,29 +3167,29 @@
         <v>2003</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="G27" t="b">
         <v>1</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I27" s="28">
         <v>37817</v>
       </c>
       <c r="J27" s="29"/>
       <c r="K27" s="33" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="L27" s="22" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3202,7 +3213,7 @@
         <v>1</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I28" s="26">
         <v>37831</v>
@@ -3211,10 +3222,10 @@
         <v>37853</v>
       </c>
       <c r="K28" s="33" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="L28" s="22" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3238,7 +3249,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I29" s="26">
         <v>37998</v>
@@ -3247,10 +3258,10 @@
         <v>38028</v>
       </c>
       <c r="K29" s="22" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="L29" s="22" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3274,17 +3285,17 @@
         <v>1</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I30" s="28">
         <v>37998</v>
       </c>
       <c r="J30" s="27"/>
       <c r="K30" s="33" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="L30" s="40" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -3304,23 +3315,23 @@
         <v>1</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="G31" t="b">
         <v>0</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I31" s="28">
         <v>38090</v>
       </c>
       <c r="J31" s="29"/>
       <c r="K31" s="33" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="L31" s="22" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3334,7 +3345,7 @@
         <v>2004</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="E32" t="b">
         <v>1</v>
@@ -3344,7 +3355,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I32" s="26">
         <v>38139</v>
@@ -3353,10 +3364,10 @@
         <v>38239</v>
       </c>
       <c r="K32" s="33" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="L32" s="22" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -3380,7 +3391,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I33" s="26">
         <v>38425</v>
@@ -3389,10 +3400,10 @@
         <v>38456</v>
       </c>
       <c r="K33" s="33" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="L33" s="22" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -3416,7 +3427,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I34" s="26">
         <v>38608</v>
@@ -3428,10 +3439,10 @@
         <v>83</v>
       </c>
       <c r="L34" s="22" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="24">
         <v>30674</v>
       </c>
@@ -3452,7 +3463,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I35" s="26">
         <v>38981</v>
@@ -3461,10 +3472,10 @@
         <v>38989</v>
       </c>
       <c r="K35" s="33" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="L35" s="22" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -3488,7 +3499,7 @@
         <v>1</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I36" s="26">
         <v>39021</v>
@@ -3497,10 +3508,10 @@
         <v>39184</v>
       </c>
       <c r="K36" s="33" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="L36" s="40" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="75" x14ac:dyDescent="0.25">
@@ -3520,13 +3531,13 @@
         <v>1</v>
       </c>
       <c r="F37" s="22" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="G37" t="b">
         <v>0</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I37" s="26">
         <v>39069</v>
@@ -3535,10 +3546,10 @@
         <v>38892</v>
       </c>
       <c r="K37" s="33" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="L37" s="40" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -3562,7 +3573,7 @@
         <v>1</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I38" s="26">
         <v>39113</v>
@@ -3571,10 +3582,10 @@
         <v>39132</v>
       </c>
       <c r="K38" s="33" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="L38" s="35" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -3598,7 +3609,7 @@
         <v>1</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I39" s="30">
         <v>39136</v>
@@ -3607,10 +3618,10 @@
         <v>39233</v>
       </c>
       <c r="K39" s="33" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="L39" s="35" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3634,7 +3645,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I40" s="26">
         <v>39287</v>
@@ -3643,10 +3654,10 @@
         <v>39357</v>
       </c>
       <c r="K40" s="33" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="L40" s="35" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3670,7 +3681,7 @@
         <v>1</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I41" s="26">
         <v>39790</v>
@@ -3679,10 +3690,10 @@
         <v>39813</v>
       </c>
       <c r="K41" s="33" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="L41" s="35" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -3706,7 +3717,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I42" s="26">
         <v>39804</v>
@@ -3715,10 +3726,10 @@
         <v>39811</v>
       </c>
       <c r="K42" s="33" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="L42" s="22" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -3742,7 +3753,7 @@
         <v>1</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I43" s="26">
         <v>39811</v>
@@ -3754,7 +3765,7 @@
         <v>83</v>
       </c>
       <c r="L43" s="22" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -3778,7 +3789,7 @@
         <v>1</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I44" s="26">
         <v>40437</v>
@@ -3787,10 +3798,10 @@
         <v>40445</v>
       </c>
       <c r="K44" s="33" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="L44" s="22" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3814,7 +3825,7 @@
         <v>1</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I45" s="26">
         <v>40450</v>
@@ -3823,10 +3834,10 @@
         <v>40515</v>
       </c>
       <c r="K45" s="33" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="L45" s="35" t="s">
-        <v>491</v>
+        <v>549</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3850,7 +3861,7 @@
         <v>1</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I46" s="26">
         <v>40491</v>
@@ -3859,10 +3870,10 @@
         <v>40529</v>
       </c>
       <c r="K46" s="33" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="L46" s="22" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="105" x14ac:dyDescent="0.25">
@@ -3882,13 +3893,13 @@
         <v>0</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="G47" t="b">
         <v>1</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I47" s="26">
         <v>40533</v>
@@ -3897,10 +3908,10 @@
         <v>41049</v>
       </c>
       <c r="K47" s="33" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="L47" s="22" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -3920,7 +3931,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="22" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="G48" t="b">
         <v>0</v>
@@ -3938,7 +3949,7 @@
         <v>83</v>
       </c>
       <c r="L48" s="22" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -3971,10 +3982,10 @@
         <v>41257</v>
       </c>
       <c r="K49" s="33" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="L49" s="22" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -3994,7 +4005,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="22" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="G50" t="b">
         <v>0</v>
@@ -4007,10 +4018,10 @@
       </c>
       <c r="J50" s="29"/>
       <c r="K50" s="33" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="L50" s="22" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -4034,7 +4045,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="I51" s="26">
         <v>43147</v>
@@ -4046,10 +4057,10 @@
         <v>83</v>
       </c>
       <c r="L51" s="22" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
         <v>416</v>
       </c>
@@ -4070,7 +4081,7 @@
         <v>1</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="I52" s="26">
         <v>43481</v>
@@ -4079,10 +4090,10 @@
         <v>43536</v>
       </c>
       <c r="K52" s="33" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="L52" s="22" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -4106,7 +4117,7 @@
         <v>1</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="I53" s="26">
         <v>43727</v>
@@ -4118,7 +4129,7 @@
         <v>83</v>
       </c>
       <c r="L53" s="22" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="75" x14ac:dyDescent="0.25">
@@ -4138,7 +4149,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="22" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="G54" t="b">
         <v>0</v>
@@ -4153,15 +4164,15 @@
         <v>43798</v>
       </c>
       <c r="K54" s="37" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="L54" s="35" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="B55" t="s">
         <v>410</v>
@@ -4179,7 +4190,7 @@
         <v>1</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="I55" s="32">
         <v>43829</v>
@@ -4188,10 +4199,10 @@
         <v>44231</v>
       </c>
       <c r="K55" s="37" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="L55" s="35" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -4214,7 +4225,7 @@
         <v>1</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="I56" s="26">
         <v>43969</v>
@@ -4226,7 +4237,7 @@
         <v>83</v>
       </c>
       <c r="L56" s="35" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -4388,10 +4399,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="B7" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -5423,7 +5434,7 @@
         <v>146</v>
       </c>
       <c r="B54" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="C54" s="5" t="b">
         <v>1</v>
@@ -6890,7 +6901,7 @@
         <v>270</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>6</v>
@@ -6911,12 +6922,12 @@
         <v>43738</v>
       </c>
       <c r="P7" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="B8" s="42">
         <v>1352</v>
@@ -6955,7 +6966,7 @@
         <v>43769</v>
       </c>
       <c r="P8" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -15405,8 +15416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14:H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15421,10 +15432,10 @@
         <v>274</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -15517,52 +15528,58 @@
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="B10" s="46">
         <v>44046</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="B11" s="46">
         <v>44049</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="B12" s="46">
         <v>44118</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="B13" s="46">
         <v>44466</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
+        <v>538</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
+        <v>546</v>
+      </c>
+      <c r="B14" s="46">
+        <v>44516</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>551</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="44"/>
@@ -15709,7 +15726,7 @@
         <v>389</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>10</v>
@@ -15729,7 +15746,7 @@
         <v>429</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>8</v>
@@ -15766,10 +15783,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>8</v>
@@ -15806,16 +15823,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="12" t="s">
+        <v>537</v>
+      </c>
+      <c r="D9" t="s">
         <v>542</v>
-      </c>
-      <c r="D9" t="s">
-        <v>547</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -15866,10 +15883,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>8</v>
@@ -15884,10 +15901,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>8</v>
@@ -16145,7 +16162,7 @@
         <v>336</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>8</v>
@@ -16245,7 +16262,7 @@
         <v>239</v>
       </c>
       <c r="D31" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>277</v>
@@ -16265,7 +16282,7 @@
         <v>238</v>
       </c>
       <c r="D32" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>277</v>
@@ -16305,7 +16322,7 @@
         <v>244</v>
       </c>
       <c r="D34" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>8</v>
@@ -16362,7 +16379,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>282</v>
@@ -16382,7 +16399,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>353</v>

</xml_diff>

<commit_message>
updated tables to v20220412
Added Biological Criteria to John Day TMDL. Added Chlorophyll a to Snake River Hells Canyon TMDLs. Changed pollutant for 1994 Coquille River TMDL from BOD to UBOD. Updated Umatilla TMDL parameters and pollutants names to Aquatic Weeds or Algae and Ammonia Nitrogen (NH3-N). Updated Rickreall Creek issue date. Added Action ID for Little River TMDL addendum. Added phosphorus to Umpqua, Upper Klamath Lake Drainage, and Upper Grande Ronde TMDL listed parameters. Added Aquatic Weeds or Algae to Upper Grande Ronde.
</commit_message>
<xml_diff>
--- a/data_raw/TMDL_db_tabular.xlsx
+++ b/data_raw/TMDL_db_tabular.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GitHub\odeqtmdl\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576DCDC6-1BFF-4431-838D-8F1FD97176A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="780" windowWidth="27075" windowHeight="13905"/>
+    <workbookView xWindow="20685" yWindow="120" windowWidth="19920" windowHeight="18780" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tmdl_actions_table" sheetId="7" r:id="rId1"/>
@@ -21,19 +22,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">geo_id_table!$A$1:$F$90</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">pollutant_table!$A$1:$P$201</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tmdl_actions_table!$A$1:$L$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tmdl_actions_table!$A$1:$N$56</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="659">
   <si>
     <t>Total Phosphorus</t>
   </si>
@@ -1109,9 +1119,6 @@
     <t>John Day River Basin TMDL and WQMP</t>
   </si>
   <si>
-    <t>Lower Grande Ronde Subbasins TMDLS</t>
-  </si>
-  <si>
     <t>TMDL_issue_year</t>
   </si>
   <si>
@@ -1286,27 +1293,15 @@
     <t>Nuisance Algal Growth, pH</t>
   </si>
   <si>
-    <t>BOD</t>
-  </si>
-  <si>
     <t>Total Phosphorus, E. coli, DDT/DDE, dieldrin, dioxin, PCBs, BOD5, Lead</t>
   </si>
   <si>
     <t>Heat</t>
   </si>
   <si>
-    <t>Dissolved Oxygen, pH, Sedimentation, Temperature</t>
-  </si>
-  <si>
     <t>Heat, Sediment, Dissolved Inorganic Nitrogen, DOP</t>
   </si>
   <si>
-    <t>Ammonia, Aquatic Weeds,  pH, Bacteria (water contact recreation), Nitrate, Sedimentation, Turbidity, Temperature</t>
-  </si>
-  <si>
-    <t>Heat, E. coli, Nitrate, Turbidity, Total Suspended Solids</t>
-  </si>
-  <si>
     <t>Bacteria (water contact recreation), Bacteria (shellfish harvesting), Temperature</t>
   </si>
   <si>
@@ -1328,18 +1323,12 @@
     <t>E. coli, fecal coliform, Sediment, Heat</t>
   </si>
   <si>
-    <t>pH, Dissolved Oxygen, Chlorophyll a, Temperature</t>
-  </si>
-  <si>
     <t>Heat, Total Phosphorus</t>
   </si>
   <si>
     <t>Total Dissolved Gas</t>
   </si>
   <si>
-    <t>Bacteria (water contact recreation), Dissolved Oxygen, Algae, pH, Sediment, Temperature, DDT, Dieldrin</t>
-  </si>
-  <si>
     <t>Total Phosphorus, Heat, DDT, Dieldrin, Total Suspended Solids, Total Dissolved Gas</t>
   </si>
   <si>
@@ -1358,9 +1347,6 @@
     <t>Bacteria (water contact recreation), DDT, dieldrin, Dissolved Oxygen, Mercury, Temperature, Turbidity</t>
   </si>
   <si>
-    <t>Algae, Dissolved Oxygen, pH, Bacteria (water contact recreation), Bacteria (shellfish harvesting), Temperature</t>
-  </si>
-  <si>
     <t>Heat, E. coli, fecal coliform, Total Phosphorus, BOD, Organic Solids, inorganic N, inorganic P, Phosphorus recycling</t>
   </si>
   <si>
@@ -1391,9 +1377,6 @@
     <t>Bacteria (water contact recreation), Dissolved Oxygen, Chlorophyll a, pH, Temperature</t>
   </si>
   <si>
-    <t>Bacteria (water contact recreation), Dissolved Oxygen, Temperature</t>
-  </si>
-  <si>
     <t>Heat, E. coli</t>
   </si>
   <si>
@@ -1706,9 +1689,6 @@
     <t>DEQ (Oregon Department of Environmental Quality). 1999. "Western Hood Subbasin Total Maximum Daily Load (TMDL)."</t>
   </si>
   <si>
-    <t>Willow Creek Subbasin Temperature, pH and Bacteria Total Maximum Daily Loads and Water Quality Management Plan</t>
-  </si>
-  <si>
     <t>DEQ (Oregon Department of Environmental Quality). 2007. "Willow Creek Subbasin Temperature, pH and Bacteria Total Maximum Daily Loads and Water Quality Management Plan."</t>
   </si>
   <si>
@@ -1998,12 +1978,54 @@
   </si>
   <si>
     <t xml:space="preserve"> Added '1991_ColumbiaDioxin_Willamette_atPortland' and '1991_ColumbiaDioxin_Columbia_belowLongview' into geo_id_table and pollutant_table. These are dioxin targets. Updated multiple TMDL document names to match the name on the cover of the TMDL document. Added fields 'citation_abbbreviated' and 'citation_full' to tmdl_actions_table.</t>
+  </si>
+  <si>
+    <t>Bacteria (water contact recreation), Biological Criteria, Dissolved Oxygen, Temperature</t>
+  </si>
+  <si>
+    <t>Bacteria (water contact recreation), Chlorphyll a, Dissolved Oxygen, Algae, pH, Sediment, Temperature, DDT, Dieldrin</t>
+  </si>
+  <si>
+    <t>329</t>
+  </si>
+  <si>
+    <t>Ultimate Biochemical Oxygen Demand</t>
+  </si>
+  <si>
+    <t>Ammonia, Aquatic Weeds or Algae,  pH, Bacteria (water contact recreation), Nitrate, Sedimentation, Turbidity, Temperature</t>
+  </si>
+  <si>
+    <t>Heat, E. coli, Nitrate, Ammonia Nitrogen (NH3-N), Turbidity, Total Suspended Solids</t>
+  </si>
+  <si>
+    <t>Algae, Dissolved Oxygen, pH, Bacteria (water contact recreation), Bacteria (shellfish harvesting), Phosphorus, Temperature</t>
+  </si>
+  <si>
+    <t>pH, Dissolved Oxygen, Chlorophyll a, Phosphorus, Temperature</t>
+  </si>
+  <si>
+    <t>pH, Algae, Phosphorus</t>
+  </si>
+  <si>
+    <t>Aquatic Weeds or Algae, Dissolved Oxygen, pH, Sedimentation, Phosphorus, Temperature</t>
+  </si>
+  <si>
+    <t>Willow Creek Subbasin Temperature, pH, and Bacteria Total Maximum Daily Loads and Water Quality Management Plan</t>
+  </si>
+  <si>
+    <t>Lower Grande Ronde Subbasins TMDLs</t>
+  </si>
+  <si>
+    <t>v20220412</t>
+  </si>
+  <si>
+    <t>Added Biological Criteria to John Day TMDL. Added Chlorophyll a to Snake River Hells Canyon TMDLs. Changed pollutant for 1994 Coquille River TMDL from BOD to UBOD. Updated Umatilla TMDL parameters and pollutants names to Aquatic Weeds or Algae and Ammonia Nitrogen (NH3-N). Updated Rickreall Creek issue date. Added Action ID for Little River TMDL addendum. Added phosphorus to Umpqua, Upper Klamath Lake Drainage, and Upper Grande Ronde TMDL listed parameters. Added Aquatic Weeds or Algae to Upper Grande Ronde.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
@@ -2501,10 +2523,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2532,40 +2556,40 @@
         <v>230</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2579,7 +2603,7 @@
         <v>1988</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -2589,7 +2613,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I2" s="28">
         <v>32408</v>
@@ -2598,16 +2622,16 @@
         <v>32423</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="L2" s="35" t="s">
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -2621,19 +2645,19 @@
         <v>1988</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I3" s="26">
         <v>32408</v>
@@ -2648,10 +2672,10 @@
         <v>42</v>
       </c>
       <c r="M3" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2659,13 +2683,13 @@
         <v>319</v>
       </c>
       <c r="B4" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="C4">
         <v>1991</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -2675,7 +2699,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I4" s="28">
         <v>33294</v>
@@ -2684,16 +2708,16 @@
         <v>33294</v>
       </c>
       <c r="K4" s="33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="L4" s="33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="M4" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2707,7 +2731,7 @@
         <v>1991</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -2717,7 +2741,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I5" s="28">
         <v>33462</v>
@@ -2726,16 +2750,16 @@
         <v>33679</v>
       </c>
       <c r="K5" s="37" t="s">
+        <v>412</v>
+      </c>
+      <c r="L5" s="37" t="s">
         <v>413</v>
       </c>
-      <c r="L5" s="37" t="s">
-        <v>414</v>
-      </c>
       <c r="M5" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -2743,13 +2767,13 @@
         <v>2038</v>
       </c>
       <c r="B6" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="C6">
         <v>1991</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -2759,7 +2783,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I6" s="28">
         <v>33462</v>
@@ -2768,16 +2792,16 @@
         <v>33679</v>
       </c>
       <c r="K6" s="33" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="L6" s="38" t="s">
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="N6" t="s">
-        <v>621</v>
+        <v>611</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -2785,13 +2809,13 @@
         <v>1352</v>
       </c>
       <c r="B7" t="s">
-        <v>540</v>
+        <v>531</v>
       </c>
       <c r="C7">
         <v>1991</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -2801,7 +2825,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I7" s="26">
         <v>33462</v>
@@ -2810,30 +2834,30 @@
         <v>33679</v>
       </c>
       <c r="K7" s="33" t="s">
-        <v>412</v>
+        <v>653</v>
       </c>
       <c r="L7" s="36" t="s">
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="N7" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="B8" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="C8">
         <v>1993</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -2843,7 +2867,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I8" s="28">
         <v>34182</v>
@@ -2855,13 +2879,13 @@
         <v>59</v>
       </c>
       <c r="L8" s="35" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="M8" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
       <c r="N8" t="s">
-        <v>623</v>
+        <v>613</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -2869,13 +2893,13 @@
         <v>2036</v>
       </c>
       <c r="B9" t="s">
-        <v>587</v>
+        <v>577</v>
       </c>
       <c r="C9">
         <v>1993</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -2885,10 +2909,10 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="I9" s="28">
-        <v>34304</v>
+        <v>34330</v>
       </c>
       <c r="J9" s="26">
         <v>34442</v>
@@ -2897,13 +2921,13 @@
         <v>59</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M9" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
       <c r="N9" t="s">
-        <v>622</v>
+        <v>612</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -2911,25 +2935,25 @@
         <v>1230</v>
       </c>
       <c r="B10" t="s">
-        <v>618</v>
+        <v>608</v>
       </c>
       <c r="C10">
         <v>1993</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I10" s="26">
         <v>34330</v>
@@ -2938,30 +2962,30 @@
         <v>34361</v>
       </c>
       <c r="K10" s="33" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="L10" s="39" t="s">
         <v>0</v>
       </c>
       <c r="M10" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
       <c r="N10" t="s">
-        <v>617</v>
+        <v>607</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="24">
-        <v>329</v>
+      <c r="A11" s="24" t="s">
+        <v>647</v>
       </c>
       <c r="B11" t="s">
-        <v>616</v>
+        <v>606</v>
       </c>
       <c r="C11">
         <v>1994</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -2971,7 +2995,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I11" s="28">
         <v>34394</v>
@@ -2983,13 +3007,13 @@
         <v>59</v>
       </c>
       <c r="L11" s="40" t="s">
-        <v>417</v>
+        <v>648</v>
       </c>
       <c r="M11" t="s">
-        <v>580</v>
+        <v>570</v>
       </c>
       <c r="N11" t="s">
-        <v>615</v>
+        <v>605</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -2997,13 +3021,13 @@
         <v>310</v>
       </c>
       <c r="B12" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="C12">
         <v>1995</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
@@ -3013,7 +3037,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I12" s="26">
         <v>34974</v>
@@ -3022,16 +3046,16 @@
         <v>35202</v>
       </c>
       <c r="K12" s="33" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="L12" s="38" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="M12" t="s">
-        <v>581</v>
+        <v>571</v>
       </c>
       <c r="N12" t="s">
-        <v>624</v>
+        <v>614</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -3039,13 +3063,13 @@
         <v>321</v>
       </c>
       <c r="B13" t="s">
-        <v>613</v>
+        <v>603</v>
       </c>
       <c r="C13">
         <v>1998</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -3055,7 +3079,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I13" s="26">
         <v>36039</v>
@@ -3064,16 +3088,16 @@
         <v>36124</v>
       </c>
       <c r="K13" s="33" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="L13" s="40" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="M13" t="s">
-        <v>582</v>
+        <v>572</v>
       </c>
       <c r="N13" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -3081,25 +3105,25 @@
         <v>2034</v>
       </c>
       <c r="B14" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
       <c r="C14">
         <v>1999</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I14" s="26">
         <v>36220</v>
@@ -3111,27 +3135,27 @@
         <v>79</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M14" s="47" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="24">
         <v>489</v>
       </c>
       <c r="B15" t="s">
-        <v>612</v>
+        <v>602</v>
       </c>
       <c r="C15">
         <v>2000</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>
@@ -3141,7 +3165,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I15" s="26">
         <v>36617</v>
@@ -3150,16 +3174,16 @@
         <v>36649</v>
       </c>
       <c r="K15" s="33" t="s">
-        <v>420</v>
+        <v>654</v>
       </c>
       <c r="L15" s="35" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="M15" t="s">
-        <v>583</v>
+        <v>573</v>
       </c>
       <c r="N15" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -3173,7 +3197,7 @@
         <v>2001</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E16" t="b">
         <v>1</v>
@@ -3183,7 +3207,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I16" s="26">
         <v>36892</v>
@@ -3195,13 +3219,13 @@
         <v>79</v>
       </c>
       <c r="L16" s="22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M16" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
       <c r="N16" t="s">
-        <v>610</v>
+        <v>600</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -3209,13 +3233,13 @@
         <v>1362</v>
       </c>
       <c r="B17" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="C17">
         <v>2001</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
@@ -3225,7 +3249,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I17" s="26">
         <v>36951</v>
@@ -3234,16 +3258,16 @@
         <v>37020</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>422</v>
-      </c>
-      <c r="L17" s="35" t="s">
-        <v>423</v>
+        <v>649</v>
+      </c>
+      <c r="L17" s="22" t="s">
+        <v>650</v>
       </c>
       <c r="M17" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -3251,13 +3275,13 @@
         <v>1380</v>
       </c>
       <c r="B18" t="s">
-        <v>605</v>
+        <v>595</v>
       </c>
       <c r="C18">
         <v>2001</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E18" t="b">
         <v>1</v>
@@ -3267,7 +3291,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I18" s="26">
         <v>37043</v>
@@ -3276,16 +3300,16 @@
         <v>37103</v>
       </c>
       <c r="K18" s="33" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="L18" s="22" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="M18" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
       <c r="N18" t="s">
-        <v>604</v>
+        <v>594</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -3293,13 +3317,13 @@
         <v>1936</v>
       </c>
       <c r="B19" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
       <c r="C19">
         <v>2001</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E19" t="b">
         <v>1</v>
@@ -3309,7 +3333,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I19" s="26">
         <v>37104</v>
@@ -3318,16 +3342,16 @@
         <v>37110</v>
       </c>
       <c r="K19" s="33" t="s">
+        <v>421</v>
+      </c>
+      <c r="L19" s="22" t="s">
         <v>426</v>
       </c>
-      <c r="L19" s="22" t="s">
-        <v>0</v>
-      </c>
       <c r="M19" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
       <c r="N19" t="s">
-        <v>602</v>
+        <v>592</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -3341,7 +3365,7 @@
         <v>2001</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E20" t="b">
         <v>1</v>
@@ -3351,7 +3375,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I20" s="26">
         <v>37226</v>
@@ -3360,16 +3384,16 @@
         <v>37285</v>
       </c>
       <c r="K20" s="33" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="L20" s="40" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="M20" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
       <c r="N20" t="s">
-        <v>594</v>
+        <v>584</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="60" x14ac:dyDescent="0.25">
@@ -3377,25 +3401,25 @@
         <v>2021</v>
       </c>
       <c r="B21" t="s">
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="C21">
         <v>2001</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I21" s="26">
         <v>37226</v>
@@ -3407,13 +3431,13 @@
         <v>79</v>
       </c>
       <c r="L21" s="22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M21" s="47" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -3421,13 +3445,13 @@
         <v>2258</v>
       </c>
       <c r="B22" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
       <c r="C22">
         <v>2002</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E22" t="b">
         <v>1</v>
@@ -3437,7 +3461,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I22" s="26">
         <v>37347</v>
@@ -3449,13 +3473,13 @@
         <v>79</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M22" s="47" t="s">
-        <v>584</v>
+        <v>574</v>
       </c>
       <c r="N22" s="13" t="s">
-        <v>570</v>
+        <v>560</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -3463,13 +3487,13 @@
         <v>2241</v>
       </c>
       <c r="B23" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
       <c r="C23">
         <v>2002</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
@@ -3479,7 +3503,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I23" s="26">
         <v>37347</v>
@@ -3491,13 +3515,13 @@
         <v>79</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M23" s="47" t="s">
-        <v>584</v>
+        <v>574</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -3505,13 +3529,13 @@
         <v>2238</v>
       </c>
       <c r="B24" t="s">
-        <v>601</v>
+        <v>591</v>
       </c>
       <c r="C24">
         <v>2002</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E24" t="b">
         <v>1</v>
@@ -3521,7 +3545,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I24" s="26">
         <v>37347</v>
@@ -3530,30 +3554,30 @@
         <v>37389</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="L24" s="40" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="M24" s="47" t="s">
-        <v>584</v>
+        <v>574</v>
       </c>
       <c r="N24" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="24">
         <v>2352</v>
       </c>
       <c r="B25" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="C25">
         <v>2002</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
@@ -3563,7 +3587,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I25" s="26">
         <v>37377</v>
@@ -3572,16 +3596,16 @@
         <v>37475</v>
       </c>
       <c r="K25" s="33" t="s">
-        <v>431</v>
+        <v>652</v>
       </c>
       <c r="L25" s="22" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="M25" s="47" t="s">
-        <v>584</v>
+        <v>574</v>
       </c>
       <c r="N25" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -3589,13 +3613,13 @@
         <v>3753</v>
       </c>
       <c r="B26" t="s">
-        <v>597</v>
+        <v>587</v>
       </c>
       <c r="C26">
         <v>2002</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>599</v>
+        <v>589</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
@@ -3605,7 +3629,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I26" s="26">
         <v>37526</v>
@@ -3614,58 +3638,58 @@
         <v>37578</v>
       </c>
       <c r="K26" s="33" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="L26" s="41" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="M26" s="47" t="s">
-        <v>598</v>
+        <v>588</v>
       </c>
       <c r="N26" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="24">
         <v>10007</v>
       </c>
       <c r="B27" t="s">
-        <v>590</v>
+        <v>580</v>
       </c>
       <c r="C27">
         <v>2003</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="G27" t="b">
         <v>1</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I27" s="28">
         <v>37817</v>
       </c>
       <c r="J27" s="29"/>
       <c r="K27" s="33" t="s">
-        <v>434</v>
+        <v>646</v>
       </c>
       <c r="L27" s="22" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="M27" t="s">
-        <v>592</v>
+        <v>582</v>
       </c>
       <c r="N27" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -3673,13 +3697,13 @@
         <v>9447</v>
       </c>
       <c r="B28" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
       <c r="C28">
         <v>2003</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
@@ -3689,7 +3713,7 @@
         <v>1</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I28" s="26">
         <v>37831</v>
@@ -3698,16 +3722,16 @@
         <v>37853</v>
       </c>
       <c r="K28" s="33" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="L28" s="22" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="M28" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="N28" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -3715,25 +3739,25 @@
         <v>9767</v>
       </c>
       <c r="B29" t="s">
-        <v>588</v>
+        <v>578</v>
       </c>
       <c r="C29">
         <v>2004</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E29" t="b">
         <v>1</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="G29" t="b">
         <v>1</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I29" s="26">
         <v>37998</v>
@@ -3742,16 +3766,16 @@
         <v>38028</v>
       </c>
       <c r="K29" s="22" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="L29" s="22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M29" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="N29" t="s">
-        <v>631</v>
+        <v>621</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -3759,13 +3783,13 @@
         <v>10006</v>
       </c>
       <c r="B30" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="C30">
         <v>2004</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -3775,79 +3799,79 @@
         <v>1</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I30" s="28">
         <v>37998</v>
       </c>
       <c r="J30" s="27"/>
       <c r="K30" s="33" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="L30" s="40" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="M30" s="47" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="N30" s="13" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>259</v>
+        <v>390</v>
       </c>
       <c r="B31" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
       <c r="C31">
         <v>2004</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="G31" t="b">
         <v>0</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I31" s="28">
         <v>38090</v>
       </c>
       <c r="J31" s="29"/>
       <c r="K31" s="33" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="L31" s="22" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="M31" s="47" t="s">
-        <v>596</v>
+        <v>586</v>
       </c>
       <c r="N31" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="24">
         <v>10791</v>
       </c>
       <c r="B32" t="s">
-        <v>590</v>
+        <v>580</v>
       </c>
       <c r="C32">
         <v>2004</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
       <c r="E32" t="b">
         <v>1</v>
@@ -3857,7 +3881,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I32" s="26">
         <v>38139</v>
@@ -3866,16 +3890,16 @@
         <v>38239</v>
       </c>
       <c r="K32" s="33" t="s">
-        <v>434</v>
+        <v>646</v>
       </c>
       <c r="L32" s="22" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="M32" t="s">
-        <v>593</v>
+        <v>583</v>
       </c>
       <c r="N32" t="s">
-        <v>632</v>
+        <v>622</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -3883,13 +3907,13 @@
         <v>11395</v>
       </c>
       <c r="B33" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
       <c r="C33">
         <v>2005</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E33" t="b">
         <v>1</v>
@@ -3899,7 +3923,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I33" s="26">
         <v>38425</v>
@@ -3908,16 +3932,16 @@
         <v>38456</v>
       </c>
       <c r="K33" s="33" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="L33" s="22" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="M33" s="47" t="s">
-        <v>644</v>
+        <v>634</v>
       </c>
       <c r="N33" s="13" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -3925,13 +3949,13 @@
         <v>12241</v>
       </c>
       <c r="B34" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
       <c r="C34">
         <v>2005</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E34" t="b">
         <v>1</v>
@@ -3941,7 +3965,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I34" s="26">
         <v>38608</v>
@@ -3953,13 +3977,13 @@
         <v>79</v>
       </c>
       <c r="L34" s="22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M34" s="47" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
       <c r="N34" s="13" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="60" x14ac:dyDescent="0.25">
@@ -3973,7 +3997,7 @@
         <v>2006</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E35" t="b">
         <v>1</v>
@@ -3983,7 +4007,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I35" s="26">
         <v>38981</v>
@@ -3992,16 +4016,16 @@
         <v>38989</v>
       </c>
       <c r="K35" s="33" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="L35" s="22" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="M35" s="47" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
       <c r="N35" s="13" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -4009,13 +4033,13 @@
         <v>30358</v>
       </c>
       <c r="B36" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="C36">
         <v>2006</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E36" t="b">
         <v>1</v>
@@ -4025,7 +4049,7 @@
         <v>1</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I36" s="26">
         <v>39021</v>
@@ -4034,42 +4058,42 @@
         <v>39184</v>
       </c>
       <c r="K36" s="33" t="s">
-        <v>441</v>
+        <v>651</v>
       </c>
       <c r="L36" s="40" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="M36" s="47" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
       <c r="N36" s="13" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B37" t="s">
-        <v>561</v>
+        <v>551</v>
       </c>
       <c r="C37">
         <v>2006</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E37" t="b">
         <v>1</v>
       </c>
       <c r="F37" s="22" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="G37" t="b">
         <v>0</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I37" s="26">
         <v>39069</v>
@@ -4078,16 +4102,16 @@
         <v>38892</v>
       </c>
       <c r="K37" s="33" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="L37" s="40" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="M37" s="47" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
       <c r="N37" t="s">
-        <v>562</v>
+        <v>552</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -4095,13 +4119,13 @@
         <v>32071</v>
       </c>
       <c r="B38" t="s">
-        <v>557</v>
+        <v>655</v>
       </c>
       <c r="C38">
         <v>2007</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E38" t="b">
         <v>1</v>
@@ -4111,7 +4135,7 @@
         <v>1</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I38" s="26">
         <v>39113</v>
@@ -4120,16 +4144,16 @@
         <v>39132</v>
       </c>
       <c r="K38" s="33" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="L38" s="35" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="M38" s="47" t="s">
-        <v>619</v>
+        <v>609</v>
       </c>
       <c r="N38" s="13" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -4137,13 +4161,13 @@
         <v>33639</v>
       </c>
       <c r="B39" t="s">
-        <v>620</v>
+        <v>610</v>
       </c>
       <c r="C39">
         <v>2007</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E39" t="b">
         <v>1</v>
@@ -4153,7 +4177,7 @@
         <v>1</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I39" s="30">
         <v>39136</v>
@@ -4162,16 +4186,16 @@
         <v>39233</v>
       </c>
       <c r="K39" s="33" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="L39" s="35" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="M39" s="47" t="s">
-        <v>619</v>
+        <v>609</v>
       </c>
       <c r="N39" s="35" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4179,13 +4203,13 @@
         <v>33829</v>
       </c>
       <c r="B40" t="s">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="C40">
         <v>2007</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E40" t="b">
         <v>1</v>
@@ -4195,7 +4219,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I40" s="26">
         <v>39287</v>
@@ -4204,16 +4228,16 @@
         <v>39357</v>
       </c>
       <c r="K40" s="33" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="L40" s="35" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="M40" s="47" t="s">
-        <v>619</v>
+        <v>609</v>
       </c>
       <c r="N40" s="13" t="s">
-        <v>648</v>
+        <v>638</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4227,7 +4251,7 @@
         <v>2008</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E41" t="b">
         <v>1</v>
@@ -4237,7 +4261,7 @@
         <v>1</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I41" s="26">
         <v>39790</v>
@@ -4246,16 +4270,16 @@
         <v>39813</v>
       </c>
       <c r="K41" s="33" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="L41" s="35" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="M41" s="47" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="N41" s="13" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -4269,7 +4293,7 @@
         <v>2008</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E42" t="b">
         <v>1</v>
@@ -4279,7 +4303,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I42" s="26">
         <v>39804</v>
@@ -4288,16 +4312,16 @@
         <v>39811</v>
       </c>
       <c r="K42" s="33" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="L42" s="22" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="M42" s="47" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="N42" s="13" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -4311,7 +4335,7 @@
         <v>2008</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E43" t="b">
         <v>1</v>
@@ -4321,7 +4345,7 @@
         <v>1</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I43" s="26">
         <v>39811</v>
@@ -4333,13 +4357,13 @@
         <v>79</v>
       </c>
       <c r="L43" s="22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M43" s="47" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="N43" s="13" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -4347,13 +4371,13 @@
         <v>39294</v>
       </c>
       <c r="B44" t="s">
-        <v>358</v>
+        <v>656</v>
       </c>
       <c r="C44">
         <v>2010</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E44" t="b">
         <v>1</v>
@@ -4363,7 +4387,7 @@
         <v>1</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I44" s="26">
         <v>40437</v>
@@ -4372,16 +4396,16 @@
         <v>40445</v>
       </c>
       <c r="K44" s="33" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="L44" s="22" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="M44" s="47" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="N44" s="13" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4395,7 +4419,7 @@
         <v>2010</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E45" t="b">
         <v>1</v>
@@ -4405,7 +4429,7 @@
         <v>1</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I45" s="26">
         <v>40450</v>
@@ -4414,16 +4438,16 @@
         <v>40515</v>
       </c>
       <c r="K45" s="33" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="L45" s="35" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="M45" s="47" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="N45" s="13" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4437,7 +4461,7 @@
         <v>2010</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E46" t="b">
         <v>1</v>
@@ -4447,7 +4471,7 @@
         <v>1</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I46" s="26">
         <v>40491</v>
@@ -4456,16 +4480,16 @@
         <v>40529</v>
       </c>
       <c r="K46" s="33" t="s">
-        <v>452</v>
+        <v>645</v>
       </c>
       <c r="L46" s="22" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="M46" s="47" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="N46" s="13" t="s">
-        <v>525</v>
+        <v>516</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="105" x14ac:dyDescent="0.25">
@@ -4473,25 +4497,25 @@
         <v>42375</v>
       </c>
       <c r="B47" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="C47">
         <v>2010</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="G47" t="b">
         <v>1</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I47" s="26">
         <v>40533</v>
@@ -4500,36 +4524,36 @@
         <v>41049</v>
       </c>
       <c r="K47" s="33" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="L47" s="22" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="M47" s="47" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="N47" s="13" t="s">
-        <v>606</v>
+        <v>596</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B48" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C48">
         <v>2011</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E48" t="b">
         <v>1</v>
       </c>
       <c r="F48" s="22" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="G48" t="b">
         <v>0</v>
@@ -4547,27 +4571,27 @@
         <v>79</v>
       </c>
       <c r="L48" s="22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M48" s="47" t="s">
-        <v>543</v>
+        <v>534</v>
       </c>
       <c r="N48" t="s">
-        <v>635</v>
+        <v>625</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B49" t="s">
-        <v>552</v>
+        <v>543</v>
       </c>
       <c r="C49">
         <v>2012</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E49" t="b">
         <v>1</v>
@@ -4586,36 +4610,36 @@
         <v>41257</v>
       </c>
       <c r="K49" s="33" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="L49" s="22" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="M49" s="47" t="s">
-        <v>544</v>
+        <v>535</v>
       </c>
       <c r="N49" t="s">
-        <v>636</v>
+        <v>626</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B50" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
       <c r="C50">
         <v>2017</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
       </c>
       <c r="F50" s="22" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="G50" t="b">
         <v>0</v>
@@ -4628,30 +4652,30 @@
       </c>
       <c r="J50" s="29"/>
       <c r="K50" s="33" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="L50" s="22" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="M50" s="47" t="s">
-        <v>545</v>
+        <v>536</v>
       </c>
       <c r="N50" t="s">
-        <v>637</v>
+        <v>627</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B51" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="C51">
         <v>2018</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E51" t="b">
         <v>1</v>
@@ -4661,7 +4685,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="I51" s="26">
         <v>43147</v>
@@ -4673,27 +4697,27 @@
         <v>79</v>
       </c>
       <c r="L51" s="22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M51" s="47" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="N51" t="s">
-        <v>553</v>
+        <v>544</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B52" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
       <c r="C52">
         <v>2019</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E52" t="b">
         <v>1</v>
@@ -4703,7 +4727,7 @@
         <v>1</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="I52" s="26">
         <v>43481</v>
@@ -4712,30 +4736,30 @@
         <v>43536</v>
       </c>
       <c r="K52" s="33" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="L52" s="22" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="M52" s="47" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
       <c r="N52" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B53" t="s">
-        <v>651</v>
+        <v>641</v>
       </c>
       <c r="C53">
         <v>2019</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E53" t="b">
         <v>1</v>
@@ -4745,7 +4769,7 @@
         <v>1</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="I53" s="26">
         <v>43727</v>
@@ -4757,33 +4781,33 @@
         <v>79</v>
       </c>
       <c r="L53" s="22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M53" s="47" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
       <c r="N53" t="s">
-        <v>649</v>
+        <v>639</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C54">
         <v>2019</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
       </c>
       <c r="F54" s="22" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="G54" t="b">
         <v>0</v>
@@ -4798,30 +4822,30 @@
         <v>43798</v>
       </c>
       <c r="K54" s="37" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="L54" s="35" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="M54" s="47" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
       <c r="N54" t="s">
-        <v>639</v>
+        <v>629</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="B55" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C55">
         <v>2019</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E55" t="b">
         <v>1</v>
@@ -4830,7 +4854,7 @@
         <v>1</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="I55" s="32">
         <v>43829</v>
@@ -4839,30 +4863,30 @@
         <v>44231</v>
       </c>
       <c r="K55" s="37" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="L55" s="35" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="M55" s="47" t="s">
-        <v>548</v>
+        <v>539</v>
       </c>
       <c r="N55" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B56" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C56">
         <v>2020</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E56" t="b">
         <v>1</v>
@@ -4871,7 +4895,7 @@
         <v>1</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="I56" s="26">
         <v>43969</v>
@@ -4883,17 +4907,17 @@
         <v>79</v>
       </c>
       <c r="L56" s="35" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M56" s="47" t="s">
-        <v>549</v>
+        <v>540</v>
       </c>
       <c r="N56" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:N56">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N56">
     <sortCondition ref="I2:I56"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4902,10 +4926,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -4933,7 +4957,7 @@
         <v>248</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>230</v>
@@ -4963,7 +4987,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B3" t="s">
         <v>87</v>
@@ -4985,7 +5009,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B4" t="s">
         <v>325</v>
@@ -5007,7 +5031,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B5" t="s">
         <v>84</v>
@@ -5029,10 +5053,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="B6" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -5051,10 +5075,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
       <c r="B7" t="s">
-        <v>538</v>
+        <v>529</v>
       </c>
       <c r="C7" s="5" t="b">
         <v>1</v>
@@ -5073,7 +5097,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B8" t="s">
         <v>123</v>
@@ -5095,10 +5119,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="B9" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -5359,7 +5383,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B21" t="s">
         <v>98</v>
@@ -5381,7 +5405,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B22" t="s">
         <v>99</v>
@@ -5403,7 +5427,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B23" t="s">
         <v>103</v>
@@ -5425,7 +5449,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B24" t="s">
         <v>100</v>
@@ -5447,7 +5471,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B25" t="s">
         <v>104</v>
@@ -5469,7 +5493,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B26" t="s">
         <v>97</v>
@@ -5491,7 +5515,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B27" t="s">
         <v>92</v>
@@ -5513,7 +5537,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B28" t="s">
         <v>93</v>
@@ -5535,7 +5559,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B29" t="s">
         <v>102</v>
@@ -5557,7 +5581,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B30" t="s">
         <v>94</v>
@@ -5579,7 +5603,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B31" t="s">
         <v>101</v>
@@ -5601,7 +5625,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B32" t="s">
         <v>160</v>
@@ -5623,7 +5647,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B33" t="s">
         <v>96</v>
@@ -5645,7 +5669,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B34" t="s">
         <v>91</v>
@@ -5667,7 +5691,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B35" t="s">
         <v>95</v>
@@ -6132,7 +6156,7 @@
         <v>140</v>
       </c>
       <c r="B56" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="C56" s="5" t="b">
         <v>1</v>
@@ -6314,7 +6338,7 @@
         <v>1</v>
       </c>
       <c r="D64" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E64">
         <f>VLOOKUP(D64,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6336,7 +6360,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E65">
         <f>VLOOKUP(D65,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6358,7 +6382,7 @@
         <v>1</v>
       </c>
       <c r="D66" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E66">
         <f>VLOOKUP(D66,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6380,7 +6404,7 @@
         <v>1</v>
       </c>
       <c r="D67" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E67">
         <f>VLOOKUP(D67,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6402,7 +6426,7 @@
         <v>1</v>
       </c>
       <c r="D68" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E68">
         <f>VLOOKUP(D68,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6424,7 +6448,7 @@
         <v>1</v>
       </c>
       <c r="D69" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E69">
         <f>VLOOKUP(D69,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6446,7 +6470,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E70">
         <f>VLOOKUP(D70,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6468,7 +6492,7 @@
         <v>1</v>
       </c>
       <c r="D71" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E71">
         <f>VLOOKUP(D71,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6490,7 +6514,7 @@
         <v>1</v>
       </c>
       <c r="D72" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E72">
         <f>VLOOKUP(D72,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6512,7 +6536,7 @@
         <v>1</v>
       </c>
       <c r="D73" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E73">
         <f>VLOOKUP(D73,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6534,7 +6558,7 @@
         <v>1</v>
       </c>
       <c r="D74" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E74">
         <f>VLOOKUP(D74,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6556,7 +6580,7 @@
         <v>1</v>
       </c>
       <c r="D75" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E75">
         <f>VLOOKUP(D75,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6578,7 +6602,7 @@
         <v>1</v>
       </c>
       <c r="D76" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E76">
         <f>VLOOKUP(D76,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6600,7 +6624,7 @@
         <v>1</v>
       </c>
       <c r="D77" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E77">
         <f>VLOOKUP(D77,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6622,7 +6646,7 @@
         <v>1</v>
       </c>
       <c r="D78" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E78">
         <f>VLOOKUP(D78,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6644,7 +6668,7 @@
         <v>1</v>
       </c>
       <c r="D79" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E79">
         <f>VLOOKUP(D79,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6666,7 +6690,7 @@
         <v>1</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E80">
         <f>VLOOKUP(D80,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6688,7 +6712,7 @@
         <v>0</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E81">
         <f>VLOOKUP(D81,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6710,7 +6734,7 @@
         <v>1</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E82">
         <f>VLOOKUP(D82,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6732,7 +6756,7 @@
         <v>1</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E83">
         <f>VLOOKUP(D83,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6754,7 +6778,7 @@
         <v>1</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E84">
         <f>VLOOKUP(D84,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6776,7 +6800,7 @@
         <v>1</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E85">
         <f>VLOOKUP(D85,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6798,7 +6822,7 @@
         <v>1</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E86">
         <f>VLOOKUP(D86,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6820,7 +6844,7 @@
         <v>0</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E87">
         <f>VLOOKUP(D87,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6842,7 +6866,7 @@
         <v>0</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E88">
         <f>VLOOKUP(D88,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6864,7 +6888,7 @@
         <v>0</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E89">
         <f>VLOOKUP(D89,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6886,7 +6910,7 @@
         <v>1</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E90">
         <f>VLOOKUP(D90,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6908,7 +6932,7 @@
         <v>0</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E91">
         <f>VLOOKUP(D91,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6930,7 +6954,7 @@
         <v>0</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E92">
         <f>VLOOKUP(D92,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6952,7 +6976,7 @@
         <v>0</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E93">
         <f>VLOOKUP(D93,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6974,7 +6998,7 @@
         <v>0</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E94">
         <f>VLOOKUP(D94,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -6996,7 +7020,7 @@
         <v>0</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E95">
         <f>VLOOKUP(D95,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -7018,7 +7042,7 @@
         <v>0</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E96">
         <f>VLOOKUP(D96,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -7040,7 +7064,7 @@
         <v>1</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E97">
         <f>VLOOKUP(D97,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -7062,7 +7086,7 @@
         <v>1</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E98">
         <f>VLOOKUP(D98,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -7084,7 +7108,7 @@
         <v>1</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E99">
         <f>VLOOKUP(D99,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -7106,7 +7130,7 @@
         <v>1</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E100">
         <f>VLOOKUP(D100,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -7128,7 +7152,7 @@
         <v>0</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E101">
         <f>VLOOKUP(D101,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -7150,7 +7174,7 @@
         <v>0</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E102">
         <f>VLOOKUP(D102,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -7172,7 +7196,7 @@
         <v>1</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E103">
         <f>VLOOKUP(D103,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -7194,7 +7218,7 @@
         <v>1</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E104">
         <f>VLOOKUP(D104,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -7216,7 +7240,7 @@
         <v>1</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E105">
         <f>VLOOKUP(D105,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -7238,7 +7262,7 @@
         <v>1</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E106">
         <f>VLOOKUP(D106,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -7260,7 +7284,7 @@
         <v>1</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E107">
         <f>VLOOKUP(D107,tmdl_actions_table!$A$2:$G$60,3,FALSE)</f>
@@ -7272,7 +7296,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G104">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G104">
     <sortCondition ref="E2:E104"/>
     <sortCondition ref="A2:A104"/>
   </sortState>
@@ -7282,7 +7306,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7317,7 +7341,7 @@
         <v>248</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>230</v>
@@ -7356,7 +7380,7 @@
         <v>238</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -7405,7 +7429,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B3">
         <f>VLOOKUP(A3,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -7446,7 +7470,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B4">
         <f>VLOOKUP(A4,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -7490,7 +7514,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B5">
         <f>VLOOKUP(A5,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -7534,7 +7558,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B6">
         <f>VLOOKUP(A6,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -7578,7 +7602,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="B7">
         <v>319</v>
@@ -7591,10 +7615,10 @@
         <v>Total Maximum Daily Loading (TMDL) for 2,3,7,8-TCDD in the Columbia River Basin</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>537</v>
+        <v>528</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>6</v>
@@ -7618,12 +7642,12 @@
         <v>51</v>
       </c>
       <c r="P7" t="s">
-        <v>536</v>
+        <v>527</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
       <c r="B8">
         <v>319</v>
@@ -7636,10 +7660,10 @@
         <v>Total Maximum Daily Loading (TMDL) for 2,3,7,8-TCDD in the Columbia River Basin</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>537</v>
+        <v>528</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>6</v>
@@ -7663,12 +7687,12 @@
         <v>51</v>
       </c>
       <c r="P8" t="s">
-        <v>536</v>
+        <v>527</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B9">
         <f>VLOOKUP(A9,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -7689,7 +7713,7 @@
         <v>264</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>6</v>
@@ -7710,12 +7734,12 @@
         <v>43738</v>
       </c>
       <c r="P9" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="B10" s="42">
         <v>1352</v>
@@ -7734,7 +7758,7 @@
         <v>264</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>6</v>
@@ -7755,7 +7779,7 @@
         <v>43769</v>
       </c>
       <c r="P10" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -9372,7 +9396,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B49">
         <f>VLOOKUP(A49,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9416,7 +9440,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B50">
         <f>VLOOKUP(A50,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9460,7 +9484,7 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B51">
         <f>VLOOKUP(A51,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9504,7 +9528,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B52">
         <f>VLOOKUP(A52,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9548,7 +9572,7 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B53">
         <f>VLOOKUP(A53,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9592,7 +9616,7 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B54">
         <f>VLOOKUP(A54,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9636,7 +9660,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B55">
         <f>VLOOKUP(A55,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9680,7 +9704,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B56">
         <f>VLOOKUP(A56,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9724,7 +9748,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B57">
         <f>VLOOKUP(A57,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9768,7 +9792,7 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B58">
         <f>VLOOKUP(A58,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9812,7 +9836,7 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B59">
         <f>VLOOKUP(A59,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9856,7 +9880,7 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B60">
         <f>VLOOKUP(A60,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9903,7 +9927,7 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B61">
         <f>VLOOKUP(A61,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9947,7 +9971,7 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B62">
         <f>VLOOKUP(A62,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -9991,7 +10015,7 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B63">
         <f>VLOOKUP(A63,geo_id_table!$A$2:$F$107,4,FALSE)</f>
@@ -16190,7 +16214,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:P198">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P198">
     <sortCondition ref="C2:C198"/>
     <sortCondition ref="A2:A198"/>
     <sortCondition ref="H2:H198"/>
@@ -16202,10 +16226,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16219,10 +16245,10 @@
         <v>268</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -16293,96 +16319,102 @@
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B8" s="46">
         <v>44034</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B9" s="46">
         <v>44039</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="B10" s="46">
         <v>44046</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="B11" s="46">
         <v>44049</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="B12" s="46">
         <v>44118</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="B13" s="46">
         <v>44466</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="B14" s="46">
         <v>44516</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
       <c r="B15" s="46">
         <v>44523</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
+        <v>644</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="44" t="s">
+        <v>657</v>
+      </c>
+      <c r="B16" s="46">
+        <v>44663</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="44"/>
@@ -16431,10 +16463,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -16470,7 +16502,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -16490,7 +16522,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -16510,16 +16542,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>10</v>
@@ -16530,36 +16562,36 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>260</v>
@@ -16570,16 +16602,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>8</v>
@@ -16590,16 +16622,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>260</v>
@@ -16610,36 +16642,36 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="D9" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>271</v>
@@ -16650,16 +16682,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>402</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>403</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>271</v>
@@ -16670,16 +16702,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>8</v>
@@ -16688,16 +16720,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>8</v>
@@ -16706,16 +16738,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>646</v>
+        <v>636</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>8</v>
@@ -16726,16 +16758,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>8</v>
@@ -16832,7 +16864,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>333</v>
@@ -16912,7 +16944,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>176</v>
@@ -16995,7 +17027,7 @@
         <v>329</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>8</v>
@@ -17095,7 +17127,7 @@
         <v>233</v>
       </c>
       <c r="D33" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>271</v>
@@ -17115,7 +17147,7 @@
         <v>232</v>
       </c>
       <c r="D34" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>271</v>
@@ -17155,7 +17187,7 @@
         <v>238</v>
       </c>
       <c r="D36" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>8</v>
@@ -17172,7 +17204,7 @@
         <v>16</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D37" t="s">
         <v>344</v>
@@ -17212,7 +17244,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>276</v>
@@ -17232,7 +17264,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>346</v>
@@ -17325,7 +17357,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F25">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F25">
     <sortCondition ref="A2:A25"/>
     <sortCondition ref="B2:B25"/>
     <sortCondition ref="C2:C25"/>

</xml_diff>

<commit_message>
updated tables to v20220830
Added geo_id for Applegate cobble embeddedness. Fixed some spelling errors and removed ammonia as a pollutant from 2007 Willow Creek TMDL. Added dissolved oxygen as a pollutant for Snake River Hells Canyon. Fixed 'citation_abbreviated' spelling error.
</commit_message>
<xml_diff>
--- a/data_raw/TMDL_db_tabular.xlsx
+++ b/data_raw/TMDL_db_tabular.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{7B68424F-EC1A-4220-BBB7-CF1EF973C635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB437875-6FC2-4BCF-AB03-6329F68CEF69}"/>
   <bookViews>
-    <workbookView xWindow="17310" yWindow="330" windowWidth="33075" windowHeight="19785" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10485" yWindow="765" windowWidth="33075" windowHeight="19785" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tmdl_actions_table" sheetId="7" r:id="rId1"/>
@@ -16389,7 +16389,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>